<commit_message>
Completing recipes in excel sheet.
</commit_message>
<xml_diff>
--- a/store/Book1.xlsx
+++ b/store/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patniaka/src/feedme-ai-meal-planner/store/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8CBBBE1C-D478-A544-9819-9ACA3D40FD72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE860CDB-D6E3-464A-A1C5-1A3C881C7E19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33600" yWindow="0" windowWidth="19160" windowHeight="21600" xr2:uid="{FA15F293-69C8-0544-96C4-130C90E27DF4}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="81">
   <si>
     <t>ID</t>
   </si>
@@ -48,9 +48,6 @@
     <t>Cuisine</t>
   </si>
   <si>
-    <t>Black bean burger</t>
-  </si>
-  <si>
     <t>Meal</t>
   </si>
   <si>
@@ -127,6 +124,159 @@
   </si>
   <si>
     <t>Chinese</t>
+  </si>
+  <si>
+    <t>Aamras</t>
+  </si>
+  <si>
+    <t>Chicken Masala Fry</t>
+  </si>
+  <si>
+    <t>Avocado Roti</t>
+  </si>
+  <si>
+    <t>Black Bean burger</t>
+  </si>
+  <si>
+    <t>Chicken Curry</t>
+  </si>
+  <si>
+    <t>Sweet Potato Roti</t>
+  </si>
+  <si>
+    <t>Khichdi</t>
+  </si>
+  <si>
+    <t>Masoor Dal</t>
+  </si>
+  <si>
+    <t>Aloo Paratha</t>
+  </si>
+  <si>
+    <t>Aloo Gobi</t>
+  </si>
+  <si>
+    <t>Alfredo Pasta</t>
+  </si>
+  <si>
+    <t>Sweet Potato Pasta</t>
+  </si>
+  <si>
+    <t>Fish Cutlets</t>
+  </si>
+  <si>
+    <t>Masala Pasta</t>
+  </si>
+  <si>
+    <t>Exclude</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Shrimp Curry</t>
+  </si>
+  <si>
+    <t>Grilled Cheese</t>
+  </si>
+  <si>
+    <t>Ghugni</t>
+  </si>
+  <si>
+    <t>Toor Daal</t>
+  </si>
+  <si>
+    <t>Rajma</t>
+  </si>
+  <si>
+    <t>Cabbage Sabzi</t>
+  </si>
+  <si>
+    <t>Moong Dal Cheela</t>
+  </si>
+  <si>
+    <t>Oats Cheela</t>
+  </si>
+  <si>
+    <t>Pav Bhaji</t>
+  </si>
+  <si>
+    <t>Tomato Rice</t>
+  </si>
+  <si>
+    <t>Fish Fry</t>
+  </si>
+  <si>
+    <t>Ambat Varan</t>
+  </si>
+  <si>
+    <t>Paneer Paratha</t>
+  </si>
+  <si>
+    <t>Cabbage Paratha</t>
+  </si>
+  <si>
+    <t>Dum Aloo</t>
+  </si>
+  <si>
+    <t>Chole</t>
+  </si>
+  <si>
+    <t>Sambar</t>
+  </si>
+  <si>
+    <t>Cream Cheese Pasta</t>
+  </si>
+  <si>
+    <t>Pizza</t>
+  </si>
+  <si>
+    <t>Spinach Avocado Pasta</t>
+  </si>
+  <si>
+    <t>Pesto Pasta</t>
+  </si>
+  <si>
+    <t>Vegetable Lasagna</t>
+  </si>
+  <si>
+    <t>Creamy Lemon Chicken Sphagetti</t>
+  </si>
+  <si>
+    <t>Mac and Cheese</t>
+  </si>
+  <si>
+    <t>Italian</t>
+  </si>
+  <si>
+    <t>Fish Tacos</t>
+  </si>
+  <si>
+    <t>Cream Cheese Chicken Taquitos</t>
+  </si>
+  <si>
+    <t>Mexican Casserole</t>
+  </si>
+  <si>
+    <t>Quesadilla</t>
+  </si>
+  <si>
+    <t>Mexican</t>
+  </si>
+  <si>
+    <t>Crispy Parmesan Roast Potatoes</t>
+  </si>
+  <si>
+    <t>Grilled Chicken Salad</t>
+  </si>
+  <si>
+    <t>Mediterranean Chickpea Salad</t>
+  </si>
+  <si>
+    <t>Greek Couscous Salad</t>
+  </si>
+  <si>
+    <t>Salad</t>
   </si>
 </sst>
 </file>
@@ -478,10 +628,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B1E9D10-B7FC-0742-A85D-EE4ECB82D4D3}">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:F66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="H48" sqref="H48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -491,7 +641,7 @@
     <col min="3" max="4" width="21.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -505,290 +655,1310 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+      <c r="F1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>33</v>
       </c>
       <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" t="s">
         <v>5</v>
       </c>
-      <c r="D3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
         <v>8</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" t="s">
         <v>5</v>
       </c>
-      <c r="D4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E5" t="s">
+        <v>45</v>
+      </c>
+      <c r="F5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+      <c r="E6" t="s">
+        <v>45</v>
+      </c>
+      <c r="F6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+      <c r="E7" t="s">
+        <v>45</v>
+      </c>
+      <c r="F7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+      <c r="F8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+      <c r="E9" t="s">
+        <v>45</v>
+      </c>
+      <c r="F9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D10" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+      <c r="E10" t="s">
+        <v>45</v>
+      </c>
+      <c r="F10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D11" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+      <c r="E11" t="s">
+        <v>45</v>
+      </c>
+      <c r="F11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D12" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+      <c r="E12" t="s">
+        <v>45</v>
+      </c>
+      <c r="F12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13" t="s">
+        <v>45</v>
+      </c>
+      <c r="F13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
         <v>19</v>
       </c>
-      <c r="C13" t="s">
-        <v>26</v>
-      </c>
-      <c r="D13" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>20</v>
-      </c>
       <c r="C14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D14" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+      <c r="E14" t="s">
+        <v>45</v>
+      </c>
+      <c r="F14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D15" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+      <c r="E15" t="s">
+        <v>45</v>
+      </c>
+      <c r="F15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D16" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+      <c r="E16" t="s">
+        <v>45</v>
+      </c>
+      <c r="F16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D17" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+      <c r="E17" t="s">
+        <v>45</v>
+      </c>
+      <c r="F17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D18" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+      <c r="E18" t="s">
+        <v>45</v>
+      </c>
+      <c r="F18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" t="s">
         <v>25</v>
       </c>
-      <c r="C19" t="s">
-        <v>26</v>
-      </c>
       <c r="D19" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+      <c r="E19" t="s">
+        <v>45</v>
+      </c>
+      <c r="F19" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C20" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D20" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+        <v>29</v>
+      </c>
+      <c r="E20" t="s">
+        <v>45</v>
+      </c>
+      <c r="F20" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
+        <v>28</v>
+      </c>
+      <c r="C21" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21" t="s">
         <v>29</v>
       </c>
-      <c r="C21" t="s">
-        <v>5</v>
-      </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
+        <v>45</v>
+      </c>
+      <c r="F21" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
         <v>30</v>
+      </c>
+      <c r="C22" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22" t="s">
+        <v>26</v>
+      </c>
+      <c r="E22" t="s">
+        <v>45</v>
+      </c>
+      <c r="F22" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>31</v>
+      </c>
+      <c r="C23" t="s">
+        <v>4</v>
+      </c>
+      <c r="D23" t="s">
+        <v>26</v>
+      </c>
+      <c r="E23" t="s">
+        <v>45</v>
+      </c>
+      <c r="F23" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>34</v>
+      </c>
+      <c r="C24" t="s">
+        <v>4</v>
+      </c>
+      <c r="D24" t="s">
+        <v>26</v>
+      </c>
+      <c r="E24" t="s">
+        <v>45</v>
+      </c>
+      <c r="F24" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>32</v>
+      </c>
+      <c r="C25" t="s">
+        <v>4</v>
+      </c>
+      <c r="D25" t="s">
+        <v>26</v>
+      </c>
+      <c r="E25" t="s">
+        <v>45</v>
+      </c>
+      <c r="F25" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>35</v>
+      </c>
+      <c r="C26" t="s">
+        <v>4</v>
+      </c>
+      <c r="D26" t="s">
+        <v>26</v>
+      </c>
+      <c r="E26" t="s">
+        <v>45</v>
+      </c>
+      <c r="F26" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>36</v>
+      </c>
+      <c r="C27" t="s">
+        <v>4</v>
+      </c>
+      <c r="D27" t="s">
+        <v>26</v>
+      </c>
+      <c r="E27" t="s">
+        <v>45</v>
+      </c>
+      <c r="F27" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>37</v>
+      </c>
+      <c r="C28" t="s">
+        <v>4</v>
+      </c>
+      <c r="D28" t="s">
+        <v>26</v>
+      </c>
+      <c r="E28" t="s">
+        <v>45</v>
+      </c>
+      <c r="F28" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>39</v>
+      </c>
+      <c r="C29" t="s">
+        <v>4</v>
+      </c>
+      <c r="D29" t="s">
+        <v>26</v>
+      </c>
+      <c r="E29" t="s">
+        <v>45</v>
+      </c>
+      <c r="F29" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>30</v>
+      </c>
+      <c r="B30" t="s">
+        <v>41</v>
+      </c>
+      <c r="C30" t="s">
+        <v>4</v>
+      </c>
+      <c r="D30" t="s">
+        <v>26</v>
+      </c>
+      <c r="E30" t="s">
+        <v>45</v>
+      </c>
+      <c r="F30" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>31</v>
+      </c>
+      <c r="B31" t="s">
+        <v>42</v>
+      </c>
+      <c r="C31" t="s">
+        <v>4</v>
+      </c>
+      <c r="D31" t="s">
+        <v>26</v>
+      </c>
+      <c r="E31" t="s">
+        <v>13</v>
+      </c>
+      <c r="F31" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>32</v>
+      </c>
+      <c r="B32" t="s">
+        <v>43</v>
+      </c>
+      <c r="C32" t="s">
+        <v>4</v>
+      </c>
+      <c r="D32" t="s">
+        <v>26</v>
+      </c>
+      <c r="E32" t="s">
+        <v>45</v>
+      </c>
+      <c r="F32" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>33</v>
+      </c>
+      <c r="B33" t="s">
+        <v>46</v>
+      </c>
+      <c r="C33" t="s">
+        <v>4</v>
+      </c>
+      <c r="D33" t="s">
+        <v>26</v>
+      </c>
+      <c r="E33" t="s">
+        <v>13</v>
+      </c>
+      <c r="F33" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>34</v>
+      </c>
+      <c r="B34" t="s">
+        <v>47</v>
+      </c>
+      <c r="C34" t="s">
+        <v>4</v>
+      </c>
+      <c r="D34" t="s">
+        <v>26</v>
+      </c>
+      <c r="E34" t="s">
+        <v>45</v>
+      </c>
+      <c r="F34" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>35</v>
+      </c>
+      <c r="B35" t="s">
+        <v>48</v>
+      </c>
+      <c r="C35" t="s">
+        <v>4</v>
+      </c>
+      <c r="D35" t="s">
+        <v>26</v>
+      </c>
+      <c r="E35" t="s">
+        <v>45</v>
+      </c>
+      <c r="F35" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>36</v>
+      </c>
+      <c r="B36" t="s">
+        <v>49</v>
+      </c>
+      <c r="C36" t="s">
+        <v>4</v>
+      </c>
+      <c r="D36" t="s">
+        <v>26</v>
+      </c>
+      <c r="E36" t="s">
+        <v>45</v>
+      </c>
+      <c r="F36" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>37</v>
+      </c>
+      <c r="B37" t="s">
+        <v>50</v>
+      </c>
+      <c r="C37" t="s">
+        <v>4</v>
+      </c>
+      <c r="D37" t="s">
+        <v>26</v>
+      </c>
+      <c r="E37" t="s">
+        <v>45</v>
+      </c>
+      <c r="F37" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>38</v>
+      </c>
+      <c r="B38" t="s">
+        <v>51</v>
+      </c>
+      <c r="C38" t="s">
+        <v>4</v>
+      </c>
+      <c r="D38" t="s">
+        <v>26</v>
+      </c>
+      <c r="E38" t="s">
+        <v>45</v>
+      </c>
+      <c r="F38" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>39</v>
+      </c>
+      <c r="B39" t="s">
+        <v>52</v>
+      </c>
+      <c r="C39" t="s">
+        <v>4</v>
+      </c>
+      <c r="D39" t="s">
+        <v>26</v>
+      </c>
+      <c r="E39" t="s">
+        <v>45</v>
+      </c>
+      <c r="F39" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>40</v>
+      </c>
+      <c r="B40" t="s">
+        <v>53</v>
+      </c>
+      <c r="C40" t="s">
+        <v>4</v>
+      </c>
+      <c r="D40" t="s">
+        <v>26</v>
+      </c>
+      <c r="E40" t="s">
+        <v>45</v>
+      </c>
+      <c r="F40" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>41</v>
+      </c>
+      <c r="B41" t="s">
+        <v>54</v>
+      </c>
+      <c r="C41" t="s">
+        <v>4</v>
+      </c>
+      <c r="D41" t="s">
+        <v>26</v>
+      </c>
+      <c r="E41" t="s">
+        <v>45</v>
+      </c>
+      <c r="F41" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>42</v>
+      </c>
+      <c r="B42" t="s">
+        <v>55</v>
+      </c>
+      <c r="C42" t="s">
+        <v>4</v>
+      </c>
+      <c r="D42" t="s">
+        <v>26</v>
+      </c>
+      <c r="E42" t="s">
+        <v>45</v>
+      </c>
+      <c r="F42" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>43</v>
+      </c>
+      <c r="B43" t="s">
+        <v>56</v>
+      </c>
+      <c r="C43" t="s">
+        <v>4</v>
+      </c>
+      <c r="D43" t="s">
+        <v>26</v>
+      </c>
+      <c r="E43" t="s">
+        <v>45</v>
+      </c>
+      <c r="F43" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>44</v>
+      </c>
+      <c r="B44" t="s">
+        <v>57</v>
+      </c>
+      <c r="C44" t="s">
+        <v>4</v>
+      </c>
+      <c r="D44" t="s">
+        <v>26</v>
+      </c>
+      <c r="E44" t="s">
+        <v>45</v>
+      </c>
+      <c r="F44" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>45</v>
+      </c>
+      <c r="B45" t="s">
+        <v>58</v>
+      </c>
+      <c r="C45" t="s">
+        <v>4</v>
+      </c>
+      <c r="D45" t="s">
+        <v>26</v>
+      </c>
+      <c r="E45" t="s">
+        <v>45</v>
+      </c>
+      <c r="F45" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>46</v>
+      </c>
+      <c r="B46" t="s">
+        <v>59</v>
+      </c>
+      <c r="C46" t="s">
+        <v>4</v>
+      </c>
+      <c r="D46" t="s">
+        <v>26</v>
+      </c>
+      <c r="E46" t="s">
+        <v>45</v>
+      </c>
+      <c r="F46" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>47</v>
+      </c>
+      <c r="B47" t="s">
+        <v>38</v>
+      </c>
+      <c r="C47" t="s">
+        <v>4</v>
+      </c>
+      <c r="D47" t="s">
+        <v>26</v>
+      </c>
+      <c r="E47" t="s">
+        <v>45</v>
+      </c>
+      <c r="F47" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>48</v>
+      </c>
+      <c r="B48" t="s">
+        <v>60</v>
+      </c>
+      <c r="C48" t="s">
+        <v>4</v>
+      </c>
+      <c r="D48" t="s">
+        <v>26</v>
+      </c>
+      <c r="E48" t="s">
+        <v>13</v>
+      </c>
+      <c r="F48" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>49</v>
+      </c>
+      <c r="B49" t="s">
+        <v>61</v>
+      </c>
+      <c r="C49" t="s">
+        <v>4</v>
+      </c>
+      <c r="D49" t="s">
+        <v>26</v>
+      </c>
+      <c r="E49" t="s">
+        <v>45</v>
+      </c>
+      <c r="F49" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>50</v>
+      </c>
+      <c r="B50" t="s">
+        <v>62</v>
+      </c>
+      <c r="C50" t="s">
+        <v>4</v>
+      </c>
+      <c r="D50" t="s">
+        <v>26</v>
+      </c>
+      <c r="E50" t="s">
+        <v>13</v>
+      </c>
+      <c r="F50" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>51</v>
+      </c>
+      <c r="B51" t="s">
+        <v>63</v>
+      </c>
+      <c r="C51" t="s">
+        <v>4</v>
+      </c>
+      <c r="D51" t="s">
+        <v>70</v>
+      </c>
+      <c r="E51" t="s">
+        <v>45</v>
+      </c>
+      <c r="F51" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>52</v>
+      </c>
+      <c r="B52" t="s">
+        <v>64</v>
+      </c>
+      <c r="C52" t="s">
+        <v>4</v>
+      </c>
+      <c r="D52" t="s">
+        <v>70</v>
+      </c>
+      <c r="E52" t="s">
+        <v>45</v>
+      </c>
+      <c r="F52" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>53</v>
+      </c>
+      <c r="B53" t="s">
+        <v>65</v>
+      </c>
+      <c r="C53" t="s">
+        <v>4</v>
+      </c>
+      <c r="D53" t="s">
+        <v>70</v>
+      </c>
+      <c r="E53" t="s">
+        <v>45</v>
+      </c>
+      <c r="F53" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>54</v>
+      </c>
+      <c r="B54" t="s">
+        <v>66</v>
+      </c>
+      <c r="C54" t="s">
+        <v>4</v>
+      </c>
+      <c r="D54" t="s">
+        <v>70</v>
+      </c>
+      <c r="E54" t="s">
+        <v>13</v>
+      </c>
+      <c r="F54" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>55</v>
+      </c>
+      <c r="B55" t="s">
+        <v>40</v>
+      </c>
+      <c r="C55" t="s">
+        <v>4</v>
+      </c>
+      <c r="D55" t="s">
+        <v>70</v>
+      </c>
+      <c r="E55" t="s">
+        <v>13</v>
+      </c>
+      <c r="F55" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>56</v>
+      </c>
+      <c r="B56" t="s">
+        <v>67</v>
+      </c>
+      <c r="C56" t="s">
+        <v>4</v>
+      </c>
+      <c r="D56" t="s">
+        <v>70</v>
+      </c>
+      <c r="E56" t="s">
+        <v>13</v>
+      </c>
+      <c r="F56" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>57</v>
+      </c>
+      <c r="B57" t="s">
+        <v>68</v>
+      </c>
+      <c r="C57" t="s">
+        <v>4</v>
+      </c>
+      <c r="D57" t="s">
+        <v>70</v>
+      </c>
+      <c r="E57" t="s">
+        <v>13</v>
+      </c>
+      <c r="F57" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>58</v>
+      </c>
+      <c r="B58" t="s">
+        <v>69</v>
+      </c>
+      <c r="C58" t="s">
+        <v>4</v>
+      </c>
+      <c r="D58" t="s">
+        <v>70</v>
+      </c>
+      <c r="E58" t="s">
+        <v>13</v>
+      </c>
+      <c r="F58" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>59</v>
+      </c>
+      <c r="B59" t="s">
+        <v>71</v>
+      </c>
+      <c r="C59" t="s">
+        <v>4</v>
+      </c>
+      <c r="D59" t="s">
+        <v>75</v>
+      </c>
+      <c r="E59" t="s">
+        <v>13</v>
+      </c>
+      <c r="F59" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>60</v>
+      </c>
+      <c r="B60" t="s">
+        <v>72</v>
+      </c>
+      <c r="C60" t="s">
+        <v>4</v>
+      </c>
+      <c r="D60" t="s">
+        <v>75</v>
+      </c>
+      <c r="E60" t="s">
+        <v>13</v>
+      </c>
+      <c r="F60" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>61</v>
+      </c>
+      <c r="B61" t="s">
+        <v>73</v>
+      </c>
+      <c r="C61" t="s">
+        <v>4</v>
+      </c>
+      <c r="D61" t="s">
+        <v>75</v>
+      </c>
+      <c r="E61" t="s">
+        <v>13</v>
+      </c>
+      <c r="F61" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>62</v>
+      </c>
+      <c r="B62" t="s">
+        <v>74</v>
+      </c>
+      <c r="C62" t="s">
+        <v>4</v>
+      </c>
+      <c r="D62" t="s">
+        <v>75</v>
+      </c>
+      <c r="E62" t="s">
+        <v>45</v>
+      </c>
+      <c r="F62" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>63</v>
+      </c>
+      <c r="B63" t="s">
+        <v>76</v>
+      </c>
+      <c r="C63" t="s">
+        <v>4</v>
+      </c>
+      <c r="D63" t="s">
+        <v>80</v>
+      </c>
+      <c r="E63" t="s">
+        <v>45</v>
+      </c>
+      <c r="F63" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <v>64</v>
+      </c>
+      <c r="B64" t="s">
+        <v>77</v>
+      </c>
+      <c r="C64" t="s">
+        <v>4</v>
+      </c>
+      <c r="D64" t="s">
+        <v>80</v>
+      </c>
+      <c r="E64" t="s">
+        <v>45</v>
+      </c>
+      <c r="F64" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A65">
+        <v>65</v>
+      </c>
+      <c r="B65" t="s">
+        <v>78</v>
+      </c>
+      <c r="C65" t="s">
+        <v>4</v>
+      </c>
+      <c r="D65" t="s">
+        <v>80</v>
+      </c>
+      <c r="E65" t="s">
+        <v>45</v>
+      </c>
+      <c r="F65" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A66">
+        <v>66</v>
+      </c>
+      <c r="B66" t="s">
+        <v>79</v>
+      </c>
+      <c r="C66" t="s">
+        <v>4</v>
+      </c>
+      <c r="D66" t="s">
+        <v>80</v>
+      </c>
+      <c r="E66" t="s">
+        <v>13</v>
+      </c>
+      <c r="F66" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>